<commit_message>
SOSMC configured and working (not robust to faults). Problem with desiredAngularVelocity and desiredAngularAcceleration resolved for RLQ-R Passive and SOSMC Passive.
</commit_message>
<xml_diff>
--- a/auxiliary_files/gartt ML5208 340KV (do drone) motor table.xlsx
+++ b/auxiliary_files/gartt ML5208 340KV (do drone) motor table.xlsx
@@ -458,11 +458,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="59810731"/>
-        <c:axId val="62270213"/>
+        <c:axId val="98068996"/>
+        <c:axId val="84963762"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="59810731"/>
+        <c:axId val="98068996"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -546,12 +546,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="62270213"/>
+        <c:crossAx val="84963762"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="62270213"/>
+        <c:axId val="84963762"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -635,7 +635,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="59810731"/>
+        <c:crossAx val="98068996"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -708,8 +708,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.420363358460416"/>
-          <c:y val="0.0278006025746371"/>
+          <c:x val="0.420360397680199"/>
+          <c:y val="0.0278120290450747"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -860,11 +860,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="73914977"/>
-        <c:axId val="45713160"/>
+        <c:axId val="26162963"/>
+        <c:axId val="34696064"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="73914977"/>
+        <c:axId val="26162963"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -910,12 +910,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45713160"/>
+        <c:crossAx val="34696064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="45713160"/>
+        <c:axId val="34696064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -961,7 +961,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73914977"/>
+        <c:crossAx val="26162963"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1178,11 +1178,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="89922052"/>
-        <c:axId val="3174731"/>
+        <c:axId val="67652718"/>
+        <c:axId val="17332542"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="89922052"/>
+        <c:axId val="67652718"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1228,12 +1228,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="3174731"/>
+        <c:crossAx val="17332542"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="3174731"/>
+        <c:axId val="17332542"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1279,7 +1279,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="89922052"/>
+        <c:crossAx val="67652718"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1496,11 +1496,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="59429336"/>
-        <c:axId val="90919743"/>
+        <c:axId val="38395582"/>
+        <c:axId val="17219037"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="59429336"/>
+        <c:axId val="38395582"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1546,12 +1546,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="90919743"/>
+        <c:crossAx val="17219037"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="90919743"/>
+        <c:axId val="17219037"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1597,7 +1597,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="59429336"/>
+        <c:crossAx val="38395582"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1629,16 +1629,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>53280</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>74880</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1440</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>83880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1094400</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>233280</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>73440</xdr:rowOff>
+      <xdr:rowOff>92520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1646,8 +1646,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4192200" y="5521680"/>
-        <a:ext cx="5660640" cy="2627640"/>
+        <a:off x="1440" y="3778200"/>
+        <a:ext cx="5689440" cy="4390200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1660,15 +1660,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1097280</xdr:colOff>
+      <xdr:colOff>1098720</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>96480</xdr:rowOff>
+      <xdr:rowOff>97920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>381240</xdr:colOff>
+      <xdr:colOff>380880</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>95040</xdr:rowOff>
+      <xdr:rowOff>94680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1676,8 +1676,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9855720" y="5543280"/>
-        <a:ext cx="10363320" cy="2627640"/>
+        <a:off x="9909000" y="5544720"/>
+        <a:ext cx="10426680" cy="2625840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1696,9 +1696,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1081800</xdr:colOff>
+      <xdr:colOff>1082160</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>103320</xdr:rowOff>
+      <xdr:rowOff>103680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1706,8 +1706,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4184640" y="2907000"/>
-        <a:ext cx="5655600" cy="2643120"/>
+        <a:off x="4208040" y="2907000"/>
+        <a:ext cx="5684400" cy="2643480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1720,15 +1720,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1089720</xdr:colOff>
+      <xdr:colOff>1091160</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>102960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>373680</xdr:colOff>
+      <xdr:colOff>373320</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>103320</xdr:rowOff>
+      <xdr:rowOff>103680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1736,8 +1736,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9848160" y="2907000"/>
-        <a:ext cx="10363320" cy="2643120"/>
+        <a:off x="9901440" y="2907000"/>
+        <a:ext cx="10426680" cy="2643480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1758,23 +1758,23 @@
   <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B38" activeCellId="0" sqref="B38"/>
+      <selection pane="topLeft" activeCell="J3" activeCellId="0" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0890688259109"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.246963562753"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.85425101214575"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.4615384615385"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.7813765182186"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="26.0526315789474"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.96356275303644"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="26.1376518218623"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="18.5303643724696"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="33.4210526315789"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="24.9514170040486"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="33.7408906882591"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="25.1740890688259"/>
     <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
finished simulation of different models for NMAC
</commit_message>
<xml_diff>
--- a/auxiliary_files/gartt ML5208 340KV (do drone) motor table.xlsx
+++ b/auxiliary_files/gartt ML5208 340KV (do drone) motor table.xlsx
@@ -96,6 +96,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -118,6 +119,7 @@
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="14"/>
@@ -458,11 +460,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="98068996"/>
-        <c:axId val="84963762"/>
+        <c:axId val="64195520"/>
+        <c:axId val="43497962"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="98068996"/>
+        <c:axId val="64195520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -546,12 +548,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84963762"/>
+        <c:crossAx val="43497962"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="84963762"/>
+        <c:axId val="43497962"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -635,7 +637,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98068996"/>
+        <c:crossAx val="64195520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -708,8 +710,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.420360397680199"/>
-          <c:y val="0.0278120290450747"/>
+          <c:x val="0.420316711590296"/>
+          <c:y val="0.0276977924036748"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -860,11 +862,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="26162963"/>
-        <c:axId val="34696064"/>
+        <c:axId val="79391171"/>
+        <c:axId val="84012700"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="26162963"/>
+        <c:axId val="79391171"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -910,12 +912,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="34696064"/>
+        <c:crossAx val="84012700"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="34696064"/>
+        <c:axId val="84012700"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -961,7 +963,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="26162963"/>
+        <c:crossAx val="79391171"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1178,11 +1180,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="67652718"/>
-        <c:axId val="17332542"/>
+        <c:axId val="51513179"/>
+        <c:axId val="89642441"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="67652718"/>
+        <c:axId val="51513179"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1228,12 +1230,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="17332542"/>
+        <c:crossAx val="89642441"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="17332542"/>
+        <c:axId val="89642441"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1279,7 +1281,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="67652718"/>
+        <c:crossAx val="51513179"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1496,11 +1498,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="38395582"/>
-        <c:axId val="17219037"/>
+        <c:axId val="28455360"/>
+        <c:axId val="98718570"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="38395582"/>
+        <c:axId val="28455360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1546,12 +1548,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="17219037"/>
+        <c:crossAx val="98718570"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="17219037"/>
+        <c:axId val="98718570"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1597,7 +1599,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="38395582"/>
+        <c:crossAx val="28455360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1636,9 +1638,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>233280</xdr:colOff>
+      <xdr:colOff>232920</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>92520</xdr:rowOff>
+      <xdr:rowOff>92160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1647,7 +1649,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="1440" y="3778200"/>
-        <a:ext cx="5689440" cy="4390200"/>
+        <a:ext cx="5717880" cy="4389840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1662,13 +1664,13 @@
       <xdr:col>7</xdr:col>
       <xdr:colOff>1098720</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>97920</xdr:rowOff>
+      <xdr:rowOff>98280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>380880</xdr:colOff>
+      <xdr:colOff>380520</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>94680</xdr:rowOff>
+      <xdr:rowOff>94320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1676,8 +1678,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9909000" y="5544720"/>
-        <a:ext cx="10426680" cy="2625840"/>
+        <a:off x="9956880" y="5545080"/>
+        <a:ext cx="10684440" cy="2625120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1696,7 +1698,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1082160</xdr:colOff>
+      <xdr:colOff>1081800</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>103680</xdr:rowOff>
     </xdr:to>
@@ -1706,8 +1708,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4208040" y="2907000"/>
-        <a:ext cx="5684400" cy="2643480"/>
+        <a:off x="4227120" y="2907000"/>
+        <a:ext cx="5712840" cy="2643480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1726,7 +1728,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>373320</xdr:colOff>
+      <xdr:colOff>372960</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>103680</xdr:rowOff>
     </xdr:to>
@@ -1736,8 +1738,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9901440" y="2907000"/>
-        <a:ext cx="10426680" cy="2643480"/>
+        <a:off x="9949320" y="2907000"/>
+        <a:ext cx="10684440" cy="2643480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1757,24 +1759,24 @@
   </sheetPr>
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J3" activeCellId="0" sqref="J3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.3522267206478"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.96356275303644"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.5668016194332"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.8906882591093"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="26.1376518218623"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="18.5303643724696"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="33.7408906882591"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="25.1740890688259"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.0688259109312"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.6761133603239"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.6194331983806"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="34.0647773279352"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="25.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Corrected the payload inertia tensor calculation
</commit_message>
<xml_diff>
--- a/auxiliary_files/gartt ML5208 340KV (do drone) motor table.xlsx
+++ b/auxiliary_files/gartt ML5208 340KV (do drone) motor table.xlsx
@@ -460,11 +460,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="64195520"/>
-        <c:axId val="43497962"/>
+        <c:axId val="14304501"/>
+        <c:axId val="35461020"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="64195520"/>
+        <c:axId val="14304501"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -548,12 +548,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43497962"/>
+        <c:crossAx val="35461020"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="43497962"/>
+        <c:axId val="35461020"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -637,7 +637,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64195520"/>
+        <c:crossAx val="14304501"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -710,8 +710,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.420316711590296"/>
-          <c:y val="0.0276977924036748"/>
+          <c:x val="0.420304873972053"/>
+          <c:y val="0.0277015907844213"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -862,11 +862,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="79391171"/>
-        <c:axId val="84012700"/>
+        <c:axId val="80542034"/>
+        <c:axId val="11828656"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="79391171"/>
+        <c:axId val="80542034"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -912,12 +912,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84012700"/>
+        <c:crossAx val="11828656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="84012700"/>
+        <c:axId val="11828656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -963,7 +963,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79391171"/>
+        <c:crossAx val="80542034"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1180,11 +1180,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="51513179"/>
-        <c:axId val="89642441"/>
+        <c:axId val="42598008"/>
+        <c:axId val="54492272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="51513179"/>
+        <c:axId val="42598008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1230,12 +1230,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="89642441"/>
+        <c:crossAx val="54492272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="89642441"/>
+        <c:axId val="54492272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1281,7 +1281,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="51513179"/>
+        <c:crossAx val="42598008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1498,11 +1498,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="28455360"/>
-        <c:axId val="98718570"/>
+        <c:axId val="45250689"/>
+        <c:axId val="94076236"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="28455360"/>
+        <c:axId val="45250689"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1548,12 +1548,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98718570"/>
+        <c:crossAx val="94076236"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="98718570"/>
+        <c:axId val="94076236"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1599,7 +1599,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="28455360"/>
+        <c:crossAx val="45250689"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1638,9 +1638,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>232920</xdr:colOff>
+      <xdr:colOff>232560</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>92160</xdr:rowOff>
+      <xdr:rowOff>91800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1649,7 +1649,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="1440" y="3778200"/>
-        <a:ext cx="5717880" cy="4389840"/>
+        <a:ext cx="5745960" cy="4389480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1668,9 +1668,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>380520</xdr:colOff>
+      <xdr:colOff>380160</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>94320</xdr:rowOff>
+      <xdr:rowOff>93960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1678,8 +1678,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9956880" y="5545080"/>
-        <a:ext cx="10684440" cy="2625120"/>
+        <a:off x="10004400" y="5545080"/>
+        <a:ext cx="10768680" cy="2624760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1691,16 +1691,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>45720</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>102960</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1014120</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>167760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1081800</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>103680</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1582920</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>6480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1708,8 +1708,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4227120" y="2907000"/>
-        <a:ext cx="5712840" cy="2643480"/>
+        <a:off x="6528960" y="3336120"/>
+        <a:ext cx="5740920" cy="2643120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1728,9 +1728,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>372960</xdr:colOff>
+      <xdr:colOff>372600</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>103680</xdr:rowOff>
+      <xdr:rowOff>103320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1738,8 +1738,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9949320" y="2907000"/>
-        <a:ext cx="10684440" cy="2643480"/>
+        <a:off x="9996840" y="2907000"/>
+        <a:ext cx="10768680" cy="2643120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1759,24 +1759,24 @@
   </sheetPr>
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.3522267206478"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.4615384615385"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.0688259109312"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.6761133603239"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.995951417004"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="19.9230769230769"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="26.3522267206478"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.6194331983806"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="34.0647773279352"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="25.3886639676113"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.7813765182186"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.1012145748988"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="26.5668016194332"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.7125506072875"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="34.3846153846154"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="25.4939271255061"/>
     <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>

</xml_diff>